<commit_message>
Update LipidLynxX_test.csv for GitHubActions
</commit_message>
<xml_diff>
--- a/test/test_output/test_convert.xlsx
+++ b/test/test_output/test_convert.xlsx
@@ -1121,12 +1121,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Cer(d18:0/26:0(3OH))</t>
+          <t>Cer(d18:0/26:0)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cer(18:0/26:0&lt;OH{3}&gt;)</t>
+          <t>Cer(18:0/26:0)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1213,12 +1213,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Cer(d18:1/26:0(3OH))</t>
+          <t>Cer(d18:0/26:0(3OH))</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Cer(18:1/26:0&lt;OH{3}&gt;)</t>
+          <t>Cer(18:0/26:0&lt;OH{3}&gt;)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1297,12 +1297,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Cer(t18:0/26:0)</t>
+          <t>Cer(d18:1/26:0(3OH))</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Cer(18:0/26:0)</t>
+          <t>Cer(18:1/26:0&lt;OH{3}&gt;)</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1381,12 +1381,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>SM(d18:1/26:0)</t>
+          <t>Cer(t18:0/26:0)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>SM(18:1/26:0)</t>
+          <t>Cer(18:0/26:0)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1457,12 +1457,12 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>MG(16:0)</t>
+          <t>SM(d18:1/26:0)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>MG(16:0)</t>
+          <t>SM(18:1/26:0)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1525,12 +1525,12 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>DG(16:0/18:2(9Z,12Z)/0:0)[iso2]</t>
+          <t>MG(16:0)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>DG(16:0/18:2&lt;{9Z,12Z}&gt;/0:0)</t>
+          <t>MG(16:0)</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1593,12 +1593,12 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
-          <t>DG(O-16:0/18:1(9Z))</t>
+          <t>DG(16:0/18:2(9Z,12Z)/0:0)[iso2]</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>DG(O-16:0/18:1&lt;{9Z}&gt;)</t>
+          <t>DG(16:0/18:2&lt;{9Z,12Z}&gt;/0:0)</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1661,12 +1661,12 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>TG(16:0/18:0/18:2(9Z,12Z))[iso6]</t>
+          <t>DG(O-16:0/18:1(9Z))</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>TG(16:0/18:0/18:2&lt;{9Z,12Z}&gt;)</t>
+          <t>DG(O-16:0/18:1&lt;{9Z}&gt;)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1729,12 +1729,12 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>TG(16:0/18:2/HETE)</t>
+          <t>TG(16:0/18:0/18:2(9Z,12Z))[iso6]</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>TG(16:0/18:2/20:4&lt;OH&gt;)</t>
+          <t>TG(16:0/18:0/18:2&lt;{9Z,12Z}&gt;)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1795,8 +1795,16 @@
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>TG(16:0/18:2/HETE)</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>TG(16:0/18:2/20:4&lt;OH&gt;)</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>LPE O-18:1</t>

</xml_diff>